<commit_message>
One of the best commit of the year
</commit_message>
<xml_diff>
--- a/Classeur devis final.xlsx
+++ b/Classeur devis final.xlsx
@@ -1,9 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="56" documentId="8_{F8C22605-5649-4A26-A692-C6B8FE10EC08}" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{54707756-A9A0-4F5D-A7D3-198A2F4694C3}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="74">
   <si>
     <t>Unité</t>
   </si>
@@ -210,6 +209,33 @@
   </si>
   <si>
     <t>TGS evenment</t>
+  </si>
+  <si>
+    <t>Place Joueur</t>
+  </si>
+  <si>
+    <t>Place Visiteur</t>
+  </si>
+  <si>
+    <t>Cash Prize</t>
+  </si>
+  <si>
+    <t>League of Legends</t>
+  </si>
+  <si>
+    <t>Hearthstone</t>
+  </si>
+  <si>
+    <t>PUBG</t>
+  </si>
+  <si>
+    <t>Rocket League</t>
+  </si>
+  <si>
+    <t>Counter Strike</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -371,7 +397,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -394,6 +420,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -525,8 +552,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2DBA69AF-70B0-459E-AE1D-ADD6B1073499}" name="Tableau1" displayName="Tableau1" ref="A1:F38" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:F38" xr:uid="{235CE7C0-C28A-489E-A226-67C469CBB080}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2DBA69AF-70B0-459E-AE1D-ADD6B1073499}" name="Tableau1" displayName="Tableau1" ref="A1:F43" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:F43" xr:uid="{235CE7C0-C28A-489E-A226-67C469CBB080}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{256E8B09-033A-4294-86DA-A14DCA278661}" name="Colonne1"/>
     <tableColumn id="2" xr3:uid="{5076C4BA-B48A-45A4-8F47-643945E953D1}" name="Unité" dataDxfId="4"/>
@@ -540,8 +567,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0F969A27-DC75-495F-A8FA-1855DFD99542}" name="Tableau2" displayName="Tableau2" ref="G1:M26" totalsRowShown="0">
-  <autoFilter ref="G1:M26" xr:uid="{0A4BE73F-88B2-43F0-B629-AFAEBAB86287}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0F969A27-DC75-495F-A8FA-1855DFD99542}" name="Tableau2" displayName="Tableau2" ref="G1:M28" totalsRowShown="0">
+  <autoFilter ref="G1:M28" xr:uid="{0A4BE73F-88B2-43F0-B629-AFAEBAB86287}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{FE4852AA-671D-48BD-90F2-3DA2BD712A0D}" name="Colonne1"/>
     <tableColumn id="2" xr3:uid="{240C908C-5C8B-4008-A7F0-905968652E50}" name="Nom"/>
@@ -878,10 +905,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M42"/>
+  <dimension ref="A1:S47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,7 +916,9 @@
     <col min="1" max="1" width="37" customWidth="1"/>
     <col min="2" max="4" width="12.5703125" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="7" max="13" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="13" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -1158,6 +1187,9 @@
       <c r="F11" s="9" t="s">
         <v>50</v>
       </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
       <c r="H11" s="2" t="s">
         <v>27</v>
       </c>
@@ -1165,8 +1197,8 @@
         <v>9</v>
       </c>
       <c r="J11" s="6">
-        <f>150*Tableau2[[#This Row],[Taillle m²]]</f>
-        <v>1350</v>
+        <f>150*Tableau2[[#This Row],[Taillle m²]]*2</f>
+        <v>2700</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -1199,10 +1231,14 @@
       <c r="H13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J13" s="6"/>
-      <c r="K13">
-        <v>4000</v>
-      </c>
+      <c r="I13" s="6">
+        <v>9</v>
+      </c>
+      <c r="J13" s="6">
+        <f>150*Tableau2[[#This Row],[Taillle m²]]</f>
+        <v>1350</v>
+      </c>
+      <c r="K13" s="6"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
@@ -1216,10 +1252,14 @@
       <c r="H14" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J14" s="6"/>
-      <c r="K14">
-        <v>3000</v>
-      </c>
+      <c r="I14" s="6">
+        <v>9</v>
+      </c>
+      <c r="J14" s="6">
+        <f>150*Tableau2[[#This Row],[Taillle m²]]</f>
+        <v>1350</v>
+      </c>
+      <c r="K14" s="6"/>
     </row>
     <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
@@ -1240,10 +1280,14 @@
       <c r="H15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J15" s="6"/>
-      <c r="K15">
-        <v>7000</v>
-      </c>
+      <c r="I15" s="6">
+        <v>9</v>
+      </c>
+      <c r="J15" s="6">
+        <f>150*Tableau2[[#This Row],[Taillle m²]]</f>
+        <v>1350</v>
+      </c>
+      <c r="K15" s="6"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
@@ -1263,15 +1307,16 @@
       <c r="H16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="6">
         <v>9</v>
       </c>
       <c r="J16" s="6">
         <f>150*Tableau2[[#This Row],[Taillle m²]]</f>
         <v>1350</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K16" s="6"/>
+    </row>
+    <row r="17" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>14</v>
       </c>
@@ -1289,12 +1334,16 @@
       <c r="H17" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J17" s="6"/>
-      <c r="K17">
-        <v>3500</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I17" s="6">
+        <v>9</v>
+      </c>
+      <c r="J17" s="6">
+        <f>150*Tableau2[[#This Row],[Taillle m²]]</f>
+        <v>1350</v>
+      </c>
+      <c r="K17" s="6"/>
+    </row>
+    <row r="18" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>15</v>
       </c>
@@ -1312,12 +1361,16 @@
       <c r="H18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J18" s="6"/>
-      <c r="K18">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I18" s="6">
+        <v>9</v>
+      </c>
+      <c r="J18" s="6">
+        <f>150*Tableau2[[#This Row],[Taillle m²]]</f>
+        <v>1350</v>
+      </c>
+      <c r="K18" s="6"/>
+    </row>
+    <row r="19" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>16</v>
       </c>
@@ -1335,12 +1388,16 @@
       <c r="H19" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J19" s="6"/>
-      <c r="K19">
-        <v>3500</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I19" s="6">
+        <v>9</v>
+      </c>
+      <c r="J19" s="6">
+        <f>150*Tableau2[[#This Row],[Taillle m²]]</f>
+        <v>1350</v>
+      </c>
+      <c r="K19" s="6"/>
+    </row>
+    <row r="20" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>17</v>
       </c>
@@ -1366,7 +1423,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>52</v>
       </c>
@@ -1392,7 +1449,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>51</v>
       </c>
@@ -1407,6 +1464,9 @@
         <v>4467.2000000000007</v>
       </c>
       <c r="F22" s="9"/>
+      <c r="G22">
+        <v>2</v>
+      </c>
       <c r="H22" s="2" t="s">
         <v>37</v>
       </c>
@@ -1414,11 +1474,11 @@
         <v>9</v>
       </c>
       <c r="J22" s="6">
-        <f>150*Tableau2[[#This Row],[Taillle m²]]</f>
-        <v>1350</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+        <f>150*Tableau2[[#This Row],[Taillle m²]]*2</f>
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>54</v>
       </c>
@@ -1433,6 +1493,9 @@
         <v>679.8</v>
       </c>
       <c r="F23" s="9"/>
+      <c r="G23">
+        <v>3</v>
+      </c>
       <c r="H23" s="2" t="s">
         <v>38</v>
       </c>
@@ -1440,11 +1503,11 @@
         <v>9</v>
       </c>
       <c r="J23" s="6">
-        <f>150*Tableau2[[#This Row],[Taillle m²]]</f>
-        <v>1350</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+        <f>150*Tableau2[[#This Row],[Taillle m²]]*3</f>
+        <v>4050</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>55</v>
       </c>
@@ -1470,7 +1533,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>56</v>
       </c>
@@ -1485,8 +1548,15 @@
         <v>7560</v>
       </c>
       <c r="F25" s="9"/>
-    </row>
-    <row r="26" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G25" s="6"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="6"/>
+    </row>
+    <row r="26" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D26" s="9"/>
       <c r="E26" s="17">
         <f>SUM(D15:D25)</f>
@@ -1495,15 +1565,28 @@
       <c r="F26" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="H26" t="s">
-        <v>40</v>
-      </c>
-      <c r="L26" s="3">
-        <f>SUM(J4:K24)</f>
-        <v>48450</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G26" s="6"/>
+      <c r="H26" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I26" s="6">
+        <v>500</v>
+      </c>
+      <c r="J26" s="6">
+        <f>10*Tableau2[[#This Row],[Taillle m²]]</f>
+        <v>5000</v>
+      </c>
+      <c r="K26" s="6"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+    </row>
+    <row r="27" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>58</v>
       </c>
@@ -1511,8 +1594,18 @@
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
       <c r="F27" s="9"/>
-    </row>
-    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
+        <v>66</v>
+      </c>
+      <c r="I27">
+        <v>2500</v>
+      </c>
+      <c r="J27">
+        <f>5*Tableau2[[#This Row],[Taillle m²]]</f>
+        <v>12500</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
         <v>57</v>
       </c>
@@ -1527,8 +1620,16 @@
         <v>22.41</v>
       </c>
       <c r="F28" s="9"/>
-    </row>
-    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>40</v>
+      </c>
+      <c r="L28" s="3">
+        <f>SUM(J4:K27)</f>
+        <v>57450</v>
+      </c>
+      <c r="M28" s="6"/>
+    </row>
+    <row r="29" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>59</v>
       </c>
@@ -1544,7 +1645,7 @@
       </c>
       <c r="F29" s="9"/>
     </row>
-    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>60</v>
       </c>
@@ -1560,7 +1661,7 @@
       </c>
       <c r="F30" s="9"/>
     </row>
-    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>61</v>
       </c>
@@ -1577,7 +1678,7 @@
       <c r="E31" s="15"/>
       <c r="F31" s="14"/>
     </row>
-    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
@@ -1586,11 +1687,11 @@
       <c r="F32" s="9"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="7" t="s">
         <v>62</v>
       </c>
       <c r="B33" s="9">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C33" s="9">
         <v>425</v>
@@ -1607,48 +1708,116 @@
       <c r="F34" s="9"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>67</v>
+      </c>
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
       <c r="F35" s="9"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>68</v>
+      </c>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="F36" s="14"/>
-    </row>
-    <row r="37" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D36" s="9">
+        <v>6000</v>
+      </c>
+      <c r="F36" s="9"/>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>69</v>
+      </c>
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="18">
-        <f>E26+E11+D33</f>
-        <v>43952.75</v>
-      </c>
-      <c r="F37" s="13"/>
+      <c r="D37" s="9">
+        <v>2600</v>
+      </c>
+      <c r="E37" s="6"/>
+      <c r="F37" s="9"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>70</v>
+      </c>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="F38" s="19"/>
+      <c r="D38" s="9">
+        <v>500</v>
+      </c>
+      <c r="E38" s="6"/>
+      <c r="F38" s="9"/>
+    </row>
+    <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9">
+        <v>2100</v>
+      </c>
+      <c r="E39" s="6"/>
+      <c r="F39" s="9"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D40" s="1"/>
-      <c r="E40" t="s">
+      <c r="A40" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9">
+        <v>3800</v>
+      </c>
+      <c r="E40" s="6"/>
+      <c r="F40" s="9"/>
+    </row>
+    <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9">
+        <f>D36+D37+D38+D39+D40</f>
+        <v>15000</v>
+      </c>
+      <c r="F41" s="14"/>
+    </row>
+    <row r="42" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="18">
+        <f>E26+E11+D33+D41</f>
+        <v>58952.75</v>
+      </c>
+      <c r="F42" s="13"/>
+    </row>
+    <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="F43" s="19"/>
+    </row>
+    <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D45" s="1"/>
+      <c r="E45" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D41" s="1"/>
-    </row>
-    <row r="42" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E42" s="4">
-        <f>L26-E37</f>
-        <v>4497.25</v>
-      </c>
-      <c r="F42" s="4" t="s">
+    <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D46" s="1"/>
+    </row>
+    <row r="47" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E47" s="4">
+        <f>L28-E42</f>
+        <v>-1502.75</v>
+      </c>
+      <c r="F47" s="4" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>